<commit_message>
Updated timeplan and added handlingsplan
</commit_message>
<xml_diff>
--- a/Tidplan/Tidplan.xlsx
+++ b/Tidplan/Tidplan.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="54">
   <si>
     <t>Datum</t>
   </si>
@@ -169,6 +169,15 @@
   </si>
   <si>
     <t>Problemformulering inför möte Universitetet</t>
+  </si>
+  <si>
+    <t>Gjort i ordning dataset</t>
+  </si>
+  <si>
+    <t>GLM analys</t>
+  </si>
+  <si>
+    <t>Diverse</t>
   </si>
 </sst>
 </file>
@@ -448,22 +457,22 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -771,7 +780,7 @@
     <sheetView topLeftCell="A2" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A2" sqref="A2"/>
-      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
+      <selection pane="bottomLeft" activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -787,7 +796,7 @@
       </c>
       <c r="C2" s="17">
         <f>SUM(C3:C125)</f>
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>1</v>
@@ -951,34 +960,72 @@
       </c>
     </row>
     <row r="14" spans="2:5">
+      <c r="B14" s="2">
+        <v>41148</v>
+      </c>
       <c r="C14" s="3">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>51</v>
+      </c>
+      <c r="E14">
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="2:5">
+      <c r="B15" s="2">
+        <v>41149</v>
+      </c>
       <c r="C15" s="3">
-        <v>0</v>
+        <v>0.5</v>
+      </c>
+      <c r="D15" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="2:5">
+      <c r="B16" s="2">
+        <v>41150</v>
+      </c>
       <c r="C16" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="3:3">
+        <v>0.5</v>
+      </c>
+      <c r="D16" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5">
+      <c r="B17" s="2">
+        <v>41151</v>
+      </c>
       <c r="C17" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="3:3">
+        <v>1</v>
+      </c>
+      <c r="D17" t="s">
+        <v>52</v>
+      </c>
+      <c r="E17">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="B18" s="2">
+        <v>41156</v>
+      </c>
       <c r="C18" s="3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="3:3">
-      <c r="C19" s="3">
-        <v>0</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="D18" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="B19" s="2"/>
+      <c r="C19" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -990,7 +1037,7 @@
   <dimension ref="A1:IF35"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="V8" sqref="V8"/>
+      <selection activeCell="AB21" sqref="AB21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1097,33 +1144,33 @@
         <v>16</v>
       </c>
       <c r="C1" s="9"/>
-      <c r="I1" s="37" t="s">
+      <c r="I1" s="33" t="s">
         <v>38</v>
       </c>
-      <c r="J1" s="37"/>
-      <c r="K1" s="37"/>
-      <c r="L1" s="37"/>
-      <c r="M1" s="37"/>
-      <c r="N1" s="37"/>
-      <c r="O1" s="38">
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="33"/>
+      <c r="N1" s="33"/>
+      <c r="O1" s="34">
         <f>32*13.5</f>
         <v>432</v>
       </c>
-      <c r="P1" s="38"/>
-      <c r="Q1" s="38"/>
-      <c r="S1" s="37" t="s">
+      <c r="P1" s="34"/>
+      <c r="Q1" s="34"/>
+      <c r="S1" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="T1" s="37"/>
-      <c r="U1" s="37"/>
-      <c r="V1" s="37"/>
-      <c r="W1" s="37"/>
-      <c r="X1" s="38">
+      <c r="T1" s="33"/>
+      <c r="U1" s="33"/>
+      <c r="V1" s="33"/>
+      <c r="W1" s="33"/>
+      <c r="X1" s="34">
         <f>IA6</f>
         <v>389</v>
       </c>
-      <c r="Y1" s="38"/>
-      <c r="Z1" s="38"/>
+      <c r="Y1" s="34"/>
+      <c r="Z1" s="34"/>
       <c r="AD1" s="29"/>
       <c r="AE1" s="29"/>
       <c r="AF1" s="29"/>
@@ -1141,20 +1188,20 @@
         <v>17</v>
       </c>
       <c r="C2" s="10"/>
-      <c r="I2" s="37" t="s">
+      <c r="I2" s="33" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="38">
+      <c r="J2" s="33"/>
+      <c r="K2" s="33"/>
+      <c r="L2" s="33"/>
+      <c r="M2" s="33"/>
+      <c r="N2" s="33"/>
+      <c r="O2" s="34">
         <f>SUM(C7:IF7)</f>
-        <v>15</v>
-      </c>
-      <c r="P2" s="38"/>
-      <c r="Q2" s="38"/>
+        <v>21</v>
+      </c>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="34"/>
     </row>
     <row r="3" spans="1:240" ht="15.75" thickBot="1">
       <c r="B3" t="s">
@@ -1163,260 +1210,260 @@
       <c r="C3" s="11"/>
     </row>
     <row r="4" spans="1:240">
-      <c r="C4" s="36" t="s">
+      <c r="C4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="34"/>
-      <c r="N4" s="34"/>
-      <c r="O4" s="34"/>
-      <c r="P4" s="34"/>
-      <c r="Q4" s="34"/>
-      <c r="R4" s="34"/>
-      <c r="S4" s="34"/>
-      <c r="T4" s="34"/>
-      <c r="U4" s="34"/>
-      <c r="V4" s="34"/>
-      <c r="W4" s="34"/>
-      <c r="X4" s="34"/>
-      <c r="Y4" s="34"/>
-      <c r="Z4" s="34"/>
-      <c r="AA4" s="34"/>
-      <c r="AB4" s="34"/>
-      <c r="AC4" s="34" t="s">
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="36"/>
+      <c r="Q4" s="36"/>
+      <c r="R4" s="36"/>
+      <c r="S4" s="36"/>
+      <c r="T4" s="36"/>
+      <c r="U4" s="36"/>
+      <c r="V4" s="36"/>
+      <c r="W4" s="36"/>
+      <c r="X4" s="36"/>
+      <c r="Y4" s="36"/>
+      <c r="Z4" s="36"/>
+      <c r="AA4" s="36"/>
+      <c r="AB4" s="36"/>
+      <c r="AC4" s="36" t="s">
         <v>4</v>
       </c>
-      <c r="AD4" s="34"/>
-      <c r="AE4" s="34"/>
-      <c r="AF4" s="34"/>
-      <c r="AG4" s="34"/>
-      <c r="AH4" s="34"/>
-      <c r="AI4" s="34"/>
-      <c r="AJ4" s="34"/>
-      <c r="AK4" s="34"/>
-      <c r="AL4" s="34"/>
-      <c r="AM4" s="34"/>
-      <c r="AN4" s="34"/>
-      <c r="AO4" s="34"/>
-      <c r="AP4" s="34"/>
-      <c r="AQ4" s="34"/>
-      <c r="AR4" s="34"/>
-      <c r="AS4" s="34"/>
-      <c r="AT4" s="34"/>
-      <c r="AU4" s="34"/>
-      <c r="AV4" s="34"/>
-      <c r="AW4" s="34"/>
-      <c r="AX4" s="34"/>
-      <c r="AY4" s="34"/>
-      <c r="AZ4" s="34"/>
-      <c r="BA4" s="34"/>
-      <c r="BB4" s="34"/>
-      <c r="BC4" s="34"/>
-      <c r="BD4" s="34"/>
-      <c r="BE4" s="34"/>
-      <c r="BF4" s="34"/>
-      <c r="BG4" s="34" t="s">
+      <c r="AD4" s="36"/>
+      <c r="AE4" s="36"/>
+      <c r="AF4" s="36"/>
+      <c r="AG4" s="36"/>
+      <c r="AH4" s="36"/>
+      <c r="AI4" s="36"/>
+      <c r="AJ4" s="36"/>
+      <c r="AK4" s="36"/>
+      <c r="AL4" s="36"/>
+      <c r="AM4" s="36"/>
+      <c r="AN4" s="36"/>
+      <c r="AO4" s="36"/>
+      <c r="AP4" s="36"/>
+      <c r="AQ4" s="36"/>
+      <c r="AR4" s="36"/>
+      <c r="AS4" s="36"/>
+      <c r="AT4" s="36"/>
+      <c r="AU4" s="36"/>
+      <c r="AV4" s="36"/>
+      <c r="AW4" s="36"/>
+      <c r="AX4" s="36"/>
+      <c r="AY4" s="36"/>
+      <c r="AZ4" s="36"/>
+      <c r="BA4" s="36"/>
+      <c r="BB4" s="36"/>
+      <c r="BC4" s="36"/>
+      <c r="BD4" s="36"/>
+      <c r="BE4" s="36"/>
+      <c r="BF4" s="36"/>
+      <c r="BG4" s="36" t="s">
         <v>6</v>
       </c>
-      <c r="BH4" s="34"/>
-      <c r="BI4" s="34"/>
-      <c r="BJ4" s="34"/>
-      <c r="BK4" s="34"/>
-      <c r="BL4" s="34"/>
-      <c r="BM4" s="34"/>
-      <c r="BN4" s="34"/>
-      <c r="BO4" s="34"/>
-      <c r="BP4" s="34"/>
-      <c r="BQ4" s="34"/>
-      <c r="BR4" s="34"/>
-      <c r="BS4" s="34"/>
-      <c r="BT4" s="34"/>
-      <c r="BU4" s="34"/>
-      <c r="BV4" s="34"/>
-      <c r="BW4" s="34"/>
-      <c r="BX4" s="34"/>
-      <c r="BY4" s="34"/>
-      <c r="BZ4" s="34"/>
-      <c r="CA4" s="34"/>
-      <c r="CB4" s="34"/>
-      <c r="CC4" s="34"/>
-      <c r="CD4" s="34"/>
-      <c r="CE4" s="34"/>
-      <c r="CF4" s="34"/>
-      <c r="CG4" s="34"/>
-      <c r="CH4" s="34"/>
-      <c r="CI4" s="34"/>
-      <c r="CJ4" s="34"/>
-      <c r="CK4" s="34"/>
-      <c r="CL4" s="34" t="s">
+      <c r="BH4" s="36"/>
+      <c r="BI4" s="36"/>
+      <c r="BJ4" s="36"/>
+      <c r="BK4" s="36"/>
+      <c r="BL4" s="36"/>
+      <c r="BM4" s="36"/>
+      <c r="BN4" s="36"/>
+      <c r="BO4" s="36"/>
+      <c r="BP4" s="36"/>
+      <c r="BQ4" s="36"/>
+      <c r="BR4" s="36"/>
+      <c r="BS4" s="36"/>
+      <c r="BT4" s="36"/>
+      <c r="BU4" s="36"/>
+      <c r="BV4" s="36"/>
+      <c r="BW4" s="36"/>
+      <c r="BX4" s="36"/>
+      <c r="BY4" s="36"/>
+      <c r="BZ4" s="36"/>
+      <c r="CA4" s="36"/>
+      <c r="CB4" s="36"/>
+      <c r="CC4" s="36"/>
+      <c r="CD4" s="36"/>
+      <c r="CE4" s="36"/>
+      <c r="CF4" s="36"/>
+      <c r="CG4" s="36"/>
+      <c r="CH4" s="36"/>
+      <c r="CI4" s="36"/>
+      <c r="CJ4" s="36"/>
+      <c r="CK4" s="36"/>
+      <c r="CL4" s="36" t="s">
         <v>7</v>
       </c>
-      <c r="CM4" s="34"/>
-      <c r="CN4" s="34"/>
-      <c r="CO4" s="34"/>
-      <c r="CP4" s="34"/>
-      <c r="CQ4" s="34"/>
-      <c r="CR4" s="34"/>
-      <c r="CS4" s="34"/>
-      <c r="CT4" s="34"/>
-      <c r="CU4" s="34"/>
-      <c r="CV4" s="34"/>
-      <c r="CW4" s="34"/>
-      <c r="CX4" s="34"/>
-      <c r="CY4" s="34"/>
-      <c r="CZ4" s="34"/>
-      <c r="DA4" s="34"/>
-      <c r="DB4" s="34"/>
-      <c r="DC4" s="34"/>
-      <c r="DD4" s="34"/>
-      <c r="DE4" s="34"/>
-      <c r="DF4" s="34"/>
-      <c r="DG4" s="34"/>
-      <c r="DH4" s="34"/>
-      <c r="DI4" s="34"/>
-      <c r="DJ4" s="34"/>
-      <c r="DK4" s="34"/>
-      <c r="DL4" s="34"/>
-      <c r="DM4" s="34"/>
-      <c r="DN4" s="34"/>
-      <c r="DO4" s="34"/>
-      <c r="DP4" s="34" t="s">
+      <c r="CM4" s="36"/>
+      <c r="CN4" s="36"/>
+      <c r="CO4" s="36"/>
+      <c r="CP4" s="36"/>
+      <c r="CQ4" s="36"/>
+      <c r="CR4" s="36"/>
+      <c r="CS4" s="36"/>
+      <c r="CT4" s="36"/>
+      <c r="CU4" s="36"/>
+      <c r="CV4" s="36"/>
+      <c r="CW4" s="36"/>
+      <c r="CX4" s="36"/>
+      <c r="CY4" s="36"/>
+      <c r="CZ4" s="36"/>
+      <c r="DA4" s="36"/>
+      <c r="DB4" s="36"/>
+      <c r="DC4" s="36"/>
+      <c r="DD4" s="36"/>
+      <c r="DE4" s="36"/>
+      <c r="DF4" s="36"/>
+      <c r="DG4" s="36"/>
+      <c r="DH4" s="36"/>
+      <c r="DI4" s="36"/>
+      <c r="DJ4" s="36"/>
+      <c r="DK4" s="36"/>
+      <c r="DL4" s="36"/>
+      <c r="DM4" s="36"/>
+      <c r="DN4" s="36"/>
+      <c r="DO4" s="36"/>
+      <c r="DP4" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="DQ4" s="34"/>
-      <c r="DR4" s="34"/>
-      <c r="DS4" s="34"/>
-      <c r="DT4" s="34"/>
-      <c r="DU4" s="34"/>
-      <c r="DV4" s="34"/>
-      <c r="DW4" s="34"/>
-      <c r="DX4" s="34"/>
-      <c r="DY4" s="34"/>
-      <c r="DZ4" s="34"/>
-      <c r="EA4" s="34"/>
-      <c r="EB4" s="34"/>
-      <c r="EC4" s="34"/>
-      <c r="ED4" s="34"/>
-      <c r="EE4" s="34"/>
-      <c r="EF4" s="34"/>
-      <c r="EG4" s="34"/>
-      <c r="EH4" s="34"/>
-      <c r="EI4" s="34"/>
-      <c r="EJ4" s="34"/>
-      <c r="EK4" s="34"/>
-      <c r="EL4" s="34"/>
-      <c r="EM4" s="34"/>
-      <c r="EN4" s="34"/>
-      <c r="EO4" s="34"/>
-      <c r="EP4" s="34"/>
-      <c r="EQ4" s="34"/>
-      <c r="ER4" s="34"/>
-      <c r="ES4" s="34"/>
-      <c r="ET4" s="34"/>
-      <c r="EU4" s="34" t="s">
+      <c r="DQ4" s="36"/>
+      <c r="DR4" s="36"/>
+      <c r="DS4" s="36"/>
+      <c r="DT4" s="36"/>
+      <c r="DU4" s="36"/>
+      <c r="DV4" s="36"/>
+      <c r="DW4" s="36"/>
+      <c r="DX4" s="36"/>
+      <c r="DY4" s="36"/>
+      <c r="DZ4" s="36"/>
+      <c r="EA4" s="36"/>
+      <c r="EB4" s="36"/>
+      <c r="EC4" s="36"/>
+      <c r="ED4" s="36"/>
+      <c r="EE4" s="36"/>
+      <c r="EF4" s="36"/>
+      <c r="EG4" s="36"/>
+      <c r="EH4" s="36"/>
+      <c r="EI4" s="36"/>
+      <c r="EJ4" s="36"/>
+      <c r="EK4" s="36"/>
+      <c r="EL4" s="36"/>
+      <c r="EM4" s="36"/>
+      <c r="EN4" s="36"/>
+      <c r="EO4" s="36"/>
+      <c r="EP4" s="36"/>
+      <c r="EQ4" s="36"/>
+      <c r="ER4" s="36"/>
+      <c r="ES4" s="36"/>
+      <c r="ET4" s="36"/>
+      <c r="EU4" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="EV4" s="34"/>
-      <c r="EW4" s="34"/>
-      <c r="EX4" s="34"/>
-      <c r="EY4" s="34"/>
-      <c r="EZ4" s="34"/>
-      <c r="FA4" s="34"/>
-      <c r="FB4" s="34"/>
-      <c r="FC4" s="34"/>
-      <c r="FD4" s="34"/>
-      <c r="FE4" s="34"/>
-      <c r="FF4" s="34"/>
-      <c r="FG4" s="34"/>
-      <c r="FH4" s="34"/>
-      <c r="FI4" s="34"/>
-      <c r="FJ4" s="34"/>
-      <c r="FK4" s="34"/>
-      <c r="FL4" s="34"/>
-      <c r="FM4" s="34"/>
-      <c r="FN4" s="34"/>
-      <c r="FO4" s="34"/>
-      <c r="FP4" s="34"/>
-      <c r="FQ4" s="34"/>
-      <c r="FR4" s="34"/>
-      <c r="FS4" s="34"/>
-      <c r="FT4" s="34"/>
-      <c r="FU4" s="34"/>
-      <c r="FV4" s="34"/>
-      <c r="FW4" s="34"/>
-      <c r="FX4" s="34"/>
-      <c r="FY4" s="34"/>
-      <c r="FZ4" s="34" t="s">
+      <c r="EV4" s="36"/>
+      <c r="EW4" s="36"/>
+      <c r="EX4" s="36"/>
+      <c r="EY4" s="36"/>
+      <c r="EZ4" s="36"/>
+      <c r="FA4" s="36"/>
+      <c r="FB4" s="36"/>
+      <c r="FC4" s="36"/>
+      <c r="FD4" s="36"/>
+      <c r="FE4" s="36"/>
+      <c r="FF4" s="36"/>
+      <c r="FG4" s="36"/>
+      <c r="FH4" s="36"/>
+      <c r="FI4" s="36"/>
+      <c r="FJ4" s="36"/>
+      <c r="FK4" s="36"/>
+      <c r="FL4" s="36"/>
+      <c r="FM4" s="36"/>
+      <c r="FN4" s="36"/>
+      <c r="FO4" s="36"/>
+      <c r="FP4" s="36"/>
+      <c r="FQ4" s="36"/>
+      <c r="FR4" s="36"/>
+      <c r="FS4" s="36"/>
+      <c r="FT4" s="36"/>
+      <c r="FU4" s="36"/>
+      <c r="FV4" s="36"/>
+      <c r="FW4" s="36"/>
+      <c r="FX4" s="36"/>
+      <c r="FY4" s="36"/>
+      <c r="FZ4" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="GA4" s="34"/>
-      <c r="GB4" s="34"/>
-      <c r="GC4" s="34"/>
-      <c r="GD4" s="34"/>
-      <c r="GE4" s="34"/>
-      <c r="GF4" s="34"/>
-      <c r="GG4" s="34"/>
-      <c r="GH4" s="34"/>
-      <c r="GI4" s="34"/>
-      <c r="GJ4" s="34"/>
-      <c r="GK4" s="34"/>
-      <c r="GL4" s="34"/>
-      <c r="GM4" s="34"/>
-      <c r="GN4" s="34"/>
-      <c r="GO4" s="34"/>
-      <c r="GP4" s="34"/>
-      <c r="GQ4" s="34"/>
-      <c r="GR4" s="34"/>
-      <c r="GS4" s="34"/>
-      <c r="GT4" s="34"/>
-      <c r="GU4" s="34"/>
-      <c r="GV4" s="34"/>
-      <c r="GW4" s="34"/>
-      <c r="GX4" s="34"/>
-      <c r="GY4" s="34"/>
-      <c r="GZ4" s="34"/>
-      <c r="HA4" s="34"/>
-      <c r="HB4" s="34" t="s">
+      <c r="GA4" s="36"/>
+      <c r="GB4" s="36"/>
+      <c r="GC4" s="36"/>
+      <c r="GD4" s="36"/>
+      <c r="GE4" s="36"/>
+      <c r="GF4" s="36"/>
+      <c r="GG4" s="36"/>
+      <c r="GH4" s="36"/>
+      <c r="GI4" s="36"/>
+      <c r="GJ4" s="36"/>
+      <c r="GK4" s="36"/>
+      <c r="GL4" s="36"/>
+      <c r="GM4" s="36"/>
+      <c r="GN4" s="36"/>
+      <c r="GO4" s="36"/>
+      <c r="GP4" s="36"/>
+      <c r="GQ4" s="36"/>
+      <c r="GR4" s="36"/>
+      <c r="GS4" s="36"/>
+      <c r="GT4" s="36"/>
+      <c r="GU4" s="36"/>
+      <c r="GV4" s="36"/>
+      <c r="GW4" s="36"/>
+      <c r="GX4" s="36"/>
+      <c r="GY4" s="36"/>
+      <c r="GZ4" s="36"/>
+      <c r="HA4" s="36"/>
+      <c r="HB4" s="36" t="s">
         <v>11</v>
       </c>
-      <c r="HC4" s="34"/>
-      <c r="HD4" s="34"/>
-      <c r="HE4" s="34"/>
-      <c r="HF4" s="34"/>
-      <c r="HG4" s="34"/>
-      <c r="HH4" s="34"/>
-      <c r="HI4" s="34"/>
-      <c r="HJ4" s="34"/>
-      <c r="HK4" s="34"/>
-      <c r="HL4" s="34"/>
-      <c r="HM4" s="34"/>
-      <c r="HN4" s="34"/>
-      <c r="HO4" s="34"/>
-      <c r="HP4" s="34"/>
-      <c r="HQ4" s="34"/>
-      <c r="HR4" s="34"/>
-      <c r="HS4" s="34"/>
-      <c r="HT4" s="34"/>
-      <c r="HU4" s="34"/>
-      <c r="HV4" s="34"/>
-      <c r="HW4" s="34"/>
-      <c r="HX4" s="34"/>
-      <c r="HY4" s="34"/>
-      <c r="HZ4" s="34"/>
-      <c r="IA4" s="34"/>
-      <c r="IB4" s="34"/>
-      <c r="IC4" s="34"/>
-      <c r="ID4" s="34"/>
-      <c r="IE4" s="34"/>
-      <c r="IF4" s="35"/>
+      <c r="HC4" s="36"/>
+      <c r="HD4" s="36"/>
+      <c r="HE4" s="36"/>
+      <c r="HF4" s="36"/>
+      <c r="HG4" s="36"/>
+      <c r="HH4" s="36"/>
+      <c r="HI4" s="36"/>
+      <c r="HJ4" s="36"/>
+      <c r="HK4" s="36"/>
+      <c r="HL4" s="36"/>
+      <c r="HM4" s="36"/>
+      <c r="HN4" s="36"/>
+      <c r="HO4" s="36"/>
+      <c r="HP4" s="36"/>
+      <c r="HQ4" s="36"/>
+      <c r="HR4" s="36"/>
+      <c r="HS4" s="36"/>
+      <c r="HT4" s="36"/>
+      <c r="HU4" s="36"/>
+      <c r="HV4" s="36"/>
+      <c r="HW4" s="36"/>
+      <c r="HX4" s="36"/>
+      <c r="HY4" s="36"/>
+      <c r="HZ4" s="36"/>
+      <c r="IA4" s="36"/>
+      <c r="IB4" s="36"/>
+      <c r="IC4" s="36"/>
+      <c r="ID4" s="36"/>
+      <c r="IE4" s="36"/>
+      <c r="IF4" s="38"/>
     </row>
     <row r="5" spans="1:240">
       <c r="C5" s="18">
@@ -2193,7 +2240,7 @@
       <c r="AC6" s="24"/>
       <c r="AD6" s="27">
         <f>SUM(X7:AD7)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AE6" s="24">
         <v>15</v>
@@ -2208,7 +2255,7 @@
       <c r="AJ6" s="24"/>
       <c r="AK6" s="27">
         <f>SUM(AE7:AK7)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL6" s="24">
         <v>12</v>
@@ -2689,15 +2736,25 @@
         <v>1</v>
       </c>
       <c r="W7" s="21"/>
-      <c r="X7" s="21"/>
-      <c r="Y7" s="21"/>
-      <c r="Z7" s="21"/>
-      <c r="AA7" s="21"/>
+      <c r="X7" s="21">
+        <v>2</v>
+      </c>
+      <c r="Y7" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="Z7" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="AA7" s="21">
+        <v>1</v>
+      </c>
       <c r="AB7" s="21"/>
       <c r="AC7" s="21"/>
       <c r="AD7" s="21"/>
       <c r="AE7" s="21"/>
-      <c r="AF7" s="21"/>
+      <c r="AF7" s="21">
+        <v>2</v>
+      </c>
       <c r="AG7" s="21"/>
       <c r="AH7" s="21"/>
       <c r="AI7" s="21"/>
@@ -2927,21 +2984,21 @@
       </c>
       <c r="D9" s="11"/>
       <c r="H9" s="7"/>
-      <c r="EM9" s="33" t="s">
+      <c r="EM9" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="EN9" s="33"/>
-      <c r="EO9" s="33"/>
-      <c r="EP9" s="33"/>
-      <c r="EQ9" s="33"/>
-      <c r="ER9" s="33"/>
-      <c r="ES9" s="33"/>
-      <c r="ET9" s="33"/>
-      <c r="EU9" s="33"/>
-      <c r="EV9" s="33"/>
-      <c r="EW9" s="33"/>
-      <c r="EX9" s="33"/>
-      <c r="EY9" s="33"/>
+      <c r="EN9" s="37"/>
+      <c r="EO9" s="37"/>
+      <c r="EP9" s="37"/>
+      <c r="EQ9" s="37"/>
+      <c r="ER9" s="37"/>
+      <c r="ES9" s="37"/>
+      <c r="ET9" s="37"/>
+      <c r="EU9" s="37"/>
+      <c r="EV9" s="37"/>
+      <c r="EW9" s="37"/>
+      <c r="EX9" s="37"/>
+      <c r="EY9" s="37"/>
     </row>
     <row r="10" spans="1:240">
       <c r="A10" s="6">
@@ -2956,21 +3013,21 @@
       <c r="D10" s="11"/>
       <c r="E10" s="8"/>
       <c r="H10" s="7"/>
-      <c r="EM10" s="33" t="s">
+      <c r="EM10" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="EN10" s="33"/>
-      <c r="EO10" s="33"/>
-      <c r="EP10" s="33"/>
-      <c r="EQ10" s="33"/>
-      <c r="ER10" s="33"/>
-      <c r="ES10" s="33"/>
-      <c r="ET10" s="33"/>
-      <c r="EU10" s="33"/>
-      <c r="EV10" s="33"/>
-      <c r="EW10" s="33"/>
-      <c r="EX10" s="33"/>
-      <c r="EY10" s="33"/>
+      <c r="EN10" s="37"/>
+      <c r="EO10" s="37"/>
+      <c r="EP10" s="37"/>
+      <c r="EQ10" s="37"/>
+      <c r="ER10" s="37"/>
+      <c r="ES10" s="37"/>
+      <c r="ET10" s="37"/>
+      <c r="EU10" s="37"/>
+      <c r="EV10" s="37"/>
+      <c r="EW10" s="37"/>
+      <c r="EX10" s="37"/>
+      <c r="EY10" s="37"/>
     </row>
     <row r="11" spans="1:240">
       <c r="A11" s="6">
@@ -2984,21 +3041,21 @@
       </c>
       <c r="D11" s="11"/>
       <c r="H11" s="7"/>
-      <c r="EM11" s="33" t="s">
+      <c r="EM11" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="EN11" s="33"/>
-      <c r="EO11" s="33"/>
-      <c r="EP11" s="33"/>
-      <c r="EQ11" s="33"/>
-      <c r="ER11" s="33"/>
-      <c r="ES11" s="33"/>
-      <c r="ET11" s="33"/>
-      <c r="EU11" s="33"/>
-      <c r="EV11" s="33"/>
-      <c r="EW11" s="33"/>
-      <c r="EX11" s="33"/>
-      <c r="EY11" s="33"/>
+      <c r="EN11" s="37"/>
+      <c r="EO11" s="37"/>
+      <c r="EP11" s="37"/>
+      <c r="EQ11" s="37"/>
+      <c r="ER11" s="37"/>
+      <c r="ES11" s="37"/>
+      <c r="ET11" s="37"/>
+      <c r="EU11" s="37"/>
+      <c r="EV11" s="37"/>
+      <c r="EW11" s="37"/>
+      <c r="EX11" s="37"/>
+      <c r="EY11" s="37"/>
     </row>
     <row r="12" spans="1:240">
       <c r="A12" s="6">
@@ -3020,21 +3077,21 @@
       <c r="S12" t="s">
         <v>33</v>
       </c>
-      <c r="EM12" s="33" t="s">
+      <c r="EM12" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="EN12" s="33"/>
-      <c r="EO12" s="33"/>
-      <c r="EP12" s="33"/>
-      <c r="EQ12" s="33"/>
-      <c r="ER12" s="33"/>
-      <c r="ES12" s="33"/>
-      <c r="ET12" s="33"/>
-      <c r="EU12" s="33"/>
-      <c r="EV12" s="33"/>
-      <c r="EW12" s="33"/>
-      <c r="EX12" s="33"/>
-      <c r="EY12" s="33"/>
+      <c r="EN12" s="37"/>
+      <c r="EO12" s="37"/>
+      <c r="EP12" s="37"/>
+      <c r="EQ12" s="37"/>
+      <c r="ER12" s="37"/>
+      <c r="ES12" s="37"/>
+      <c r="ET12" s="37"/>
+      <c r="EU12" s="37"/>
+      <c r="EV12" s="37"/>
+      <c r="EW12" s="37"/>
+      <c r="EX12" s="37"/>
+      <c r="EY12" s="37"/>
     </row>
     <row r="13" spans="1:240">
       <c r="A13" s="6">
@@ -3047,39 +3104,39 @@
       <c r="H13" s="8"/>
       <c r="J13" s="9"/>
       <c r="V13" s="10"/>
-      <c r="EM13" s="33" t="s">
+      <c r="EM13" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="EN13" s="33"/>
-      <c r="EO13" s="33"/>
-      <c r="EP13" s="33"/>
-      <c r="EQ13" s="33"/>
-      <c r="ER13" s="33"/>
-      <c r="ES13" s="33"/>
-      <c r="ET13" s="33"/>
-      <c r="EU13" s="33"/>
-      <c r="EV13" s="33"/>
-      <c r="EW13" s="33"/>
-      <c r="EX13" s="33"/>
-      <c r="EY13" s="33"/>
+      <c r="EN13" s="37"/>
+      <c r="EO13" s="37"/>
+      <c r="EP13" s="37"/>
+      <c r="EQ13" s="37"/>
+      <c r="ER13" s="37"/>
+      <c r="ES13" s="37"/>
+      <c r="ET13" s="37"/>
+      <c r="EU13" s="37"/>
+      <c r="EV13" s="37"/>
+      <c r="EW13" s="37"/>
+      <c r="EX13" s="37"/>
+      <c r="EY13" s="37"/>
     </row>
     <row r="14" spans="1:240">
       <c r="A14" s="6"/>
-      <c r="EM14" s="33" t="s">
+      <c r="EM14" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="EN14" s="33"/>
-      <c r="EO14" s="33"/>
-      <c r="EP14" s="33"/>
-      <c r="EQ14" s="33"/>
-      <c r="ER14" s="33"/>
-      <c r="ES14" s="33"/>
-      <c r="ET14" s="33"/>
-      <c r="EU14" s="33"/>
-      <c r="EV14" s="33"/>
-      <c r="EW14" s="33"/>
-      <c r="EX14" s="33"/>
-      <c r="EY14" s="33"/>
+      <c r="EN14" s="37"/>
+      <c r="EO14" s="37"/>
+      <c r="EP14" s="37"/>
+      <c r="EQ14" s="37"/>
+      <c r="ER14" s="37"/>
+      <c r="ES14" s="37"/>
+      <c r="ET14" s="37"/>
+      <c r="EU14" s="37"/>
+      <c r="EV14" s="37"/>
+      <c r="EW14" s="37"/>
+      <c r="EX14" s="37"/>
+      <c r="EY14" s="37"/>
     </row>
     <row r="15" spans="1:240">
       <c r="A15" s="6">
@@ -3118,21 +3175,21 @@
       <c r="Z15" s="13"/>
       <c r="AA15" s="13"/>
       <c r="AB15" s="15"/>
-      <c r="EM15" s="33" t="s">
+      <c r="EM15" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="EN15" s="33"/>
-      <c r="EO15" s="33"/>
-      <c r="EP15" s="33"/>
-      <c r="EQ15" s="33"/>
-      <c r="ER15" s="33"/>
-      <c r="ES15" s="33"/>
-      <c r="ET15" s="33"/>
-      <c r="EU15" s="33"/>
-      <c r="EV15" s="33"/>
-      <c r="EW15" s="33"/>
-      <c r="EX15" s="33"/>
-      <c r="EY15" s="33"/>
+      <c r="EN15" s="37"/>
+      <c r="EO15" s="37"/>
+      <c r="EP15" s="37"/>
+      <c r="EQ15" s="37"/>
+      <c r="ER15" s="37"/>
+      <c r="ES15" s="37"/>
+      <c r="ET15" s="37"/>
+      <c r="EU15" s="37"/>
+      <c r="EV15" s="37"/>
+      <c r="EW15" s="37"/>
+      <c r="EX15" s="37"/>
+      <c r="EY15" s="37"/>
     </row>
     <row r="16" spans="1:240">
       <c r="A16" s="6">
@@ -3143,39 +3200,39 @@
       </c>
       <c r="Q16" s="9"/>
       <c r="AB16" s="12"/>
-      <c r="EM16" s="33" t="s">
+      <c r="EM16" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="EN16" s="33"/>
-      <c r="EO16" s="33"/>
-      <c r="EP16" s="33"/>
-      <c r="EQ16" s="33"/>
-      <c r="ER16" s="33"/>
-      <c r="ES16" s="33"/>
-      <c r="ET16" s="33"/>
-      <c r="EU16" s="33"/>
-      <c r="EV16" s="33"/>
-      <c r="EW16" s="33"/>
-      <c r="EX16" s="33"/>
-      <c r="EY16" s="33"/>
+      <c r="EN16" s="37"/>
+      <c r="EO16" s="37"/>
+      <c r="EP16" s="37"/>
+      <c r="EQ16" s="37"/>
+      <c r="ER16" s="37"/>
+      <c r="ES16" s="37"/>
+      <c r="ET16" s="37"/>
+      <c r="EU16" s="37"/>
+      <c r="EV16" s="37"/>
+      <c r="EW16" s="37"/>
+      <c r="EX16" s="37"/>
+      <c r="EY16" s="37"/>
     </row>
     <row r="17" spans="1:240">
       <c r="A17" s="6"/>
-      <c r="EM17" s="33" t="s">
+      <c r="EM17" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="EN17" s="33"/>
-      <c r="EO17" s="33"/>
-      <c r="EP17" s="33"/>
-      <c r="EQ17" s="33"/>
-      <c r="ER17" s="33"/>
-      <c r="ES17" s="33"/>
-      <c r="ET17" s="33"/>
-      <c r="EU17" s="33"/>
-      <c r="EV17" s="33"/>
-      <c r="EW17" s="33"/>
-      <c r="EX17" s="33"/>
-      <c r="EY17" s="33"/>
+      <c r="EN17" s="37"/>
+      <c r="EO17" s="37"/>
+      <c r="EP17" s="37"/>
+      <c r="EQ17" s="37"/>
+      <c r="ER17" s="37"/>
+      <c r="ES17" s="37"/>
+      <c r="ET17" s="37"/>
+      <c r="EU17" s="37"/>
+      <c r="EV17" s="37"/>
+      <c r="EW17" s="37"/>
+      <c r="EX17" s="37"/>
+      <c r="EY17" s="37"/>
     </row>
     <row r="18" spans="1:240">
       <c r="A18" s="6">
@@ -3241,39 +3298,39 @@
       <c r="AW18" s="13"/>
       <c r="AX18" s="13"/>
       <c r="AY18" s="16"/>
-      <c r="EM18" s="33" t="s">
+      <c r="EM18" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="EN18" s="33"/>
-      <c r="EO18" s="33"/>
-      <c r="EP18" s="33"/>
-      <c r="EQ18" s="33"/>
-      <c r="ER18" s="33"/>
-      <c r="ES18" s="33"/>
-      <c r="ET18" s="33"/>
-      <c r="EU18" s="33"/>
-      <c r="EV18" s="33"/>
-      <c r="EW18" s="33"/>
-      <c r="EX18" s="33"/>
-      <c r="EY18" s="33"/>
+      <c r="EN18" s="37"/>
+      <c r="EO18" s="37"/>
+      <c r="EP18" s="37"/>
+      <c r="EQ18" s="37"/>
+      <c r="ER18" s="37"/>
+      <c r="ES18" s="37"/>
+      <c r="ET18" s="37"/>
+      <c r="EU18" s="37"/>
+      <c r="EV18" s="37"/>
+      <c r="EW18" s="37"/>
+      <c r="EX18" s="37"/>
+      <c r="EY18" s="37"/>
     </row>
     <row r="19" spans="1:240">
       <c r="A19" s="6"/>
-      <c r="EM19" s="33" t="s">
+      <c r="EM19" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="EN19" s="33"/>
-      <c r="EO19" s="33"/>
-      <c r="EP19" s="33"/>
-      <c r="EQ19" s="33"/>
-      <c r="ER19" s="33"/>
-      <c r="ES19" s="33"/>
-      <c r="ET19" s="33"/>
-      <c r="EU19" s="33"/>
-      <c r="EV19" s="33"/>
-      <c r="EW19" s="33"/>
-      <c r="EX19" s="33"/>
-      <c r="EY19" s="33"/>
+      <c r="EN19" s="37"/>
+      <c r="EO19" s="37"/>
+      <c r="EP19" s="37"/>
+      <c r="EQ19" s="37"/>
+      <c r="ER19" s="37"/>
+      <c r="ES19" s="37"/>
+      <c r="ET19" s="37"/>
+      <c r="EU19" s="37"/>
+      <c r="EV19" s="37"/>
+      <c r="EW19" s="37"/>
+      <c r="EX19" s="37"/>
+      <c r="EY19" s="37"/>
     </row>
     <row r="20" spans="1:240">
       <c r="A20" s="6">
@@ -3303,15 +3360,21 @@
       <c r="U20" s="13"/>
       <c r="V20" s="13"/>
       <c r="W20" s="13"/>
-      <c r="X20" s="13"/>
+      <c r="X20" s="13" t="s">
+        <v>33</v>
+      </c>
       <c r="Y20" s="13"/>
       <c r="Z20" s="13"/>
-      <c r="AA20" s="13"/>
+      <c r="AA20" s="13" t="s">
+        <v>33</v>
+      </c>
       <c r="AB20" s="13"/>
       <c r="AC20" s="13"/>
       <c r="AD20" s="13"/>
       <c r="AE20" s="13"/>
-      <c r="AF20" s="13"/>
+      <c r="AF20" s="13" t="s">
+        <v>33</v>
+      </c>
       <c r="AG20" s="13"/>
       <c r="AH20" s="13"/>
       <c r="AI20" s="13"/>
@@ -3422,21 +3485,21 @@
       <c r="EJ20" s="13"/>
       <c r="EK20" s="13"/>
       <c r="EL20" s="13"/>
-      <c r="EM20" s="33" t="s">
+      <c r="EM20" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="EN20" s="33"/>
-      <c r="EO20" s="33"/>
-      <c r="EP20" s="33"/>
-      <c r="EQ20" s="33"/>
-      <c r="ER20" s="33"/>
-      <c r="ES20" s="33"/>
-      <c r="ET20" s="33"/>
-      <c r="EU20" s="33"/>
-      <c r="EV20" s="33"/>
-      <c r="EW20" s="33"/>
-      <c r="EX20" s="33"/>
-      <c r="EY20" s="33"/>
+      <c r="EN20" s="37"/>
+      <c r="EO20" s="37"/>
+      <c r="EP20" s="37"/>
+      <c r="EQ20" s="37"/>
+      <c r="ER20" s="37"/>
+      <c r="ES20" s="37"/>
+      <c r="ET20" s="37"/>
+      <c r="EU20" s="37"/>
+      <c r="EV20" s="37"/>
+      <c r="EW20" s="37"/>
+      <c r="EX20" s="37"/>
+      <c r="EY20" s="37"/>
     </row>
     <row r="21" spans="1:240">
       <c r="A21" s="6">
@@ -3447,21 +3510,21 @@
       </c>
       <c r="AZ21" s="9"/>
       <c r="EL21" s="7"/>
-      <c r="EM21" s="33" t="s">
+      <c r="EM21" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="EN21" s="33"/>
-      <c r="EO21" s="33"/>
-      <c r="EP21" s="33"/>
-      <c r="EQ21" s="33"/>
-      <c r="ER21" s="33"/>
-      <c r="ES21" s="33"/>
-      <c r="ET21" s="33"/>
-      <c r="EU21" s="33"/>
-      <c r="EV21" s="33"/>
-      <c r="EW21" s="33"/>
-      <c r="EX21" s="33"/>
-      <c r="EY21" s="33"/>
+      <c r="EN21" s="37"/>
+      <c r="EO21" s="37"/>
+      <c r="EP21" s="37"/>
+      <c r="EQ21" s="37"/>
+      <c r="ER21" s="37"/>
+      <c r="ES21" s="37"/>
+      <c r="ET21" s="37"/>
+      <c r="EU21" s="37"/>
+      <c r="EV21" s="37"/>
+      <c r="EW21" s="37"/>
+      <c r="EX21" s="37"/>
+      <c r="EY21" s="37"/>
     </row>
     <row r="22" spans="1:240">
       <c r="A22" s="6">
@@ -3472,21 +3535,21 @@
       </c>
       <c r="AZ22" s="9"/>
       <c r="EL22" s="7"/>
-      <c r="EM22" s="33" t="s">
+      <c r="EM22" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="EN22" s="33"/>
-      <c r="EO22" s="33"/>
-      <c r="EP22" s="33"/>
-      <c r="EQ22" s="33"/>
-      <c r="ER22" s="33"/>
-      <c r="ES22" s="33"/>
-      <c r="ET22" s="33"/>
-      <c r="EU22" s="33"/>
-      <c r="EV22" s="33"/>
-      <c r="EW22" s="33"/>
-      <c r="EX22" s="33"/>
-      <c r="EY22" s="33"/>
+      <c r="EN22" s="37"/>
+      <c r="EO22" s="37"/>
+      <c r="EP22" s="37"/>
+      <c r="EQ22" s="37"/>
+      <c r="ER22" s="37"/>
+      <c r="ES22" s="37"/>
+      <c r="ET22" s="37"/>
+      <c r="EU22" s="37"/>
+      <c r="EV22" s="37"/>
+      <c r="EW22" s="37"/>
+      <c r="EX22" s="37"/>
+      <c r="EY22" s="37"/>
     </row>
     <row r="23" spans="1:240">
       <c r="A23" s="6">
@@ -3497,39 +3560,39 @@
       </c>
       <c r="AZ23" s="9"/>
       <c r="EL23" s="7"/>
-      <c r="EM23" s="33" t="s">
+      <c r="EM23" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="EN23" s="33"/>
-      <c r="EO23" s="33"/>
-      <c r="EP23" s="33"/>
-      <c r="EQ23" s="33"/>
-      <c r="ER23" s="33"/>
-      <c r="ES23" s="33"/>
-      <c r="ET23" s="33"/>
-      <c r="EU23" s="33"/>
-      <c r="EV23" s="33"/>
-      <c r="EW23" s="33"/>
-      <c r="EX23" s="33"/>
-      <c r="EY23" s="33"/>
+      <c r="EN23" s="37"/>
+      <c r="EO23" s="37"/>
+      <c r="EP23" s="37"/>
+      <c r="EQ23" s="37"/>
+      <c r="ER23" s="37"/>
+      <c r="ES23" s="37"/>
+      <c r="ET23" s="37"/>
+      <c r="EU23" s="37"/>
+      <c r="EV23" s="37"/>
+      <c r="EW23" s="37"/>
+      <c r="EX23" s="37"/>
+      <c r="EY23" s="37"/>
     </row>
     <row r="24" spans="1:240">
       <c r="A24" s="6"/>
-      <c r="EM24" s="33" t="s">
+      <c r="EM24" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="EN24" s="33"/>
-      <c r="EO24" s="33"/>
-      <c r="EP24" s="33"/>
-      <c r="EQ24" s="33"/>
-      <c r="ER24" s="33"/>
-      <c r="ES24" s="33"/>
-      <c r="ET24" s="33"/>
-      <c r="EU24" s="33"/>
-      <c r="EV24" s="33"/>
-      <c r="EW24" s="33"/>
-      <c r="EX24" s="33"/>
-      <c r="EY24" s="33"/>
+      <c r="EN24" s="37"/>
+      <c r="EO24" s="37"/>
+      <c r="EP24" s="37"/>
+      <c r="EQ24" s="37"/>
+      <c r="ER24" s="37"/>
+      <c r="ES24" s="37"/>
+      <c r="ET24" s="37"/>
+      <c r="EU24" s="37"/>
+      <c r="EV24" s="37"/>
+      <c r="EW24" s="37"/>
+      <c r="EX24" s="37"/>
+      <c r="EY24" s="37"/>
     </row>
     <row r="25" spans="1:240">
       <c r="A25" s="6">
@@ -3678,21 +3741,21 @@
       <c r="EJ25" s="13"/>
       <c r="EK25" s="13"/>
       <c r="EL25" s="13"/>
-      <c r="EM25" s="33" t="s">
+      <c r="EM25" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="EN25" s="33"/>
-      <c r="EO25" s="33"/>
-      <c r="EP25" s="33"/>
-      <c r="EQ25" s="33"/>
-      <c r="ER25" s="33"/>
-      <c r="ES25" s="33"/>
-      <c r="ET25" s="33"/>
-      <c r="EU25" s="33"/>
-      <c r="EV25" s="33"/>
-      <c r="EW25" s="33"/>
-      <c r="EX25" s="33"/>
-      <c r="EY25" s="33"/>
+      <c r="EN25" s="37"/>
+      <c r="EO25" s="37"/>
+      <c r="EP25" s="37"/>
+      <c r="EQ25" s="37"/>
+      <c r="ER25" s="37"/>
+      <c r="ES25" s="37"/>
+      <c r="ET25" s="37"/>
+      <c r="EU25" s="37"/>
+      <c r="EV25" s="37"/>
+      <c r="EW25" s="37"/>
+      <c r="EX25" s="37"/>
+      <c r="EY25" s="37"/>
       <c r="EZ25" s="14"/>
       <c r="FA25" s="13"/>
       <c r="FB25" s="13"/>
@@ -3729,40 +3792,40 @@
       <c r="B26" t="s">
         <v>29</v>
       </c>
-      <c r="EM26" s="33" t="s">
+      <c r="EM26" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="EN26" s="33"/>
-      <c r="EO26" s="33"/>
-      <c r="EP26" s="33"/>
-      <c r="EQ26" s="33"/>
-      <c r="ER26" s="33"/>
-      <c r="ES26" s="33"/>
-      <c r="ET26" s="33"/>
-      <c r="EU26" s="33"/>
-      <c r="EV26" s="33"/>
-      <c r="EW26" s="33"/>
-      <c r="EX26" s="33"/>
-      <c r="EY26" s="33"/>
+      <c r="EN26" s="37"/>
+      <c r="EO26" s="37"/>
+      <c r="EP26" s="37"/>
+      <c r="EQ26" s="37"/>
+      <c r="ER26" s="37"/>
+      <c r="ES26" s="37"/>
+      <c r="ET26" s="37"/>
+      <c r="EU26" s="37"/>
+      <c r="EV26" s="37"/>
+      <c r="EW26" s="37"/>
+      <c r="EX26" s="37"/>
+      <c r="EY26" s="37"/>
       <c r="EZ26" s="9"/>
       <c r="GA26" s="7"/>
     </row>
     <row r="27" spans="1:240">
-      <c r="EM27" s="33" t="s">
+      <c r="EM27" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="EN27" s="33"/>
-      <c r="EO27" s="33"/>
-      <c r="EP27" s="33"/>
-      <c r="EQ27" s="33"/>
-      <c r="ER27" s="33"/>
-      <c r="ES27" s="33"/>
-      <c r="ET27" s="33"/>
-      <c r="EU27" s="33"/>
-      <c r="EV27" s="33"/>
-      <c r="EW27" s="33"/>
-      <c r="EX27" s="33"/>
-      <c r="EY27" s="33"/>
+      <c r="EN27" s="37"/>
+      <c r="EO27" s="37"/>
+      <c r="EP27" s="37"/>
+      <c r="EQ27" s="37"/>
+      <c r="ER27" s="37"/>
+      <c r="ES27" s="37"/>
+      <c r="ET27" s="37"/>
+      <c r="EU27" s="37"/>
+      <c r="EV27" s="37"/>
+      <c r="EW27" s="37"/>
+      <c r="EX27" s="37"/>
+      <c r="EY27" s="37"/>
     </row>
     <row r="28" spans="1:240">
       <c r="A28" s="6">
@@ -3911,21 +3974,21 @@
       <c r="EJ28" s="13"/>
       <c r="EK28" s="13"/>
       <c r="EL28" s="13"/>
-      <c r="EM28" s="33" t="s">
+      <c r="EM28" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="EN28" s="33"/>
-      <c r="EO28" s="33"/>
-      <c r="EP28" s="33"/>
-      <c r="EQ28" s="33"/>
-      <c r="ER28" s="33"/>
-      <c r="ES28" s="33"/>
-      <c r="ET28" s="33"/>
-      <c r="EU28" s="33"/>
-      <c r="EV28" s="33"/>
-      <c r="EW28" s="33"/>
-      <c r="EX28" s="33"/>
-      <c r="EY28" s="33"/>
+      <c r="EN28" s="37"/>
+      <c r="EO28" s="37"/>
+      <c r="EP28" s="37"/>
+      <c r="EQ28" s="37"/>
+      <c r="ER28" s="37"/>
+      <c r="ES28" s="37"/>
+      <c r="ET28" s="37"/>
+      <c r="EU28" s="37"/>
+      <c r="EV28" s="37"/>
+      <c r="EW28" s="37"/>
+      <c r="EX28" s="37"/>
+      <c r="EY28" s="37"/>
       <c r="EZ28" s="14"/>
       <c r="FA28" s="13"/>
       <c r="FB28" s="13"/>
@@ -3999,21 +4062,21 @@
       <c r="HR28" s="16"/>
     </row>
     <row r="29" spans="1:240">
-      <c r="EM29" s="33" t="s">
+      <c r="EM29" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="EN29" s="33"/>
-      <c r="EO29" s="33"/>
-      <c r="EP29" s="33"/>
-      <c r="EQ29" s="33"/>
-      <c r="ER29" s="33"/>
-      <c r="ES29" s="33"/>
-      <c r="ET29" s="33"/>
-      <c r="EU29" s="33"/>
-      <c r="EV29" s="33"/>
-      <c r="EW29" s="33"/>
-      <c r="EX29" s="33"/>
-      <c r="EY29" s="33"/>
+      <c r="EN29" s="37"/>
+      <c r="EO29" s="37"/>
+      <c r="EP29" s="37"/>
+      <c r="EQ29" s="37"/>
+      <c r="ER29" s="37"/>
+      <c r="ES29" s="37"/>
+      <c r="ET29" s="37"/>
+      <c r="EU29" s="37"/>
+      <c r="EV29" s="37"/>
+      <c r="EW29" s="37"/>
+      <c r="EX29" s="37"/>
+      <c r="EY29" s="37"/>
     </row>
     <row r="30" spans="1:240">
       <c r="A30" s="6">
@@ -4162,21 +4225,21 @@
       <c r="EJ30" s="13"/>
       <c r="EK30" s="13"/>
       <c r="EL30" s="13"/>
-      <c r="EM30" s="33" t="s">
+      <c r="EM30" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="EN30" s="33"/>
-      <c r="EO30" s="33"/>
-      <c r="EP30" s="33"/>
-      <c r="EQ30" s="33"/>
-      <c r="ER30" s="33"/>
-      <c r="ES30" s="33"/>
-      <c r="ET30" s="33"/>
-      <c r="EU30" s="33"/>
-      <c r="EV30" s="33"/>
-      <c r="EW30" s="33"/>
-      <c r="EX30" s="33"/>
-      <c r="EY30" s="33"/>
+      <c r="EN30" s="37"/>
+      <c r="EO30" s="37"/>
+      <c r="EP30" s="37"/>
+      <c r="EQ30" s="37"/>
+      <c r="ER30" s="37"/>
+      <c r="ES30" s="37"/>
+      <c r="ET30" s="37"/>
+      <c r="EU30" s="37"/>
+      <c r="EV30" s="37"/>
+      <c r="EW30" s="37"/>
+      <c r="EX30" s="37"/>
+      <c r="EY30" s="37"/>
       <c r="EZ30" s="13"/>
       <c r="FA30" s="13"/>
       <c r="FB30" s="13"/>
@@ -4264,103 +4327,109 @@
       <c r="IF30" s="16"/>
     </row>
     <row r="31" spans="1:240">
-      <c r="EM31" s="33" t="s">
+      <c r="EM31" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="EN31" s="33"/>
-      <c r="EO31" s="33"/>
-      <c r="EP31" s="33"/>
-      <c r="EQ31" s="33"/>
-      <c r="ER31" s="33"/>
-      <c r="ES31" s="33"/>
-      <c r="ET31" s="33"/>
-      <c r="EU31" s="33"/>
-      <c r="EV31" s="33"/>
-      <c r="EW31" s="33"/>
-      <c r="EX31" s="33"/>
-      <c r="EY31" s="33"/>
+      <c r="EN31" s="37"/>
+      <c r="EO31" s="37"/>
+      <c r="EP31" s="37"/>
+      <c r="EQ31" s="37"/>
+      <c r="ER31" s="37"/>
+      <c r="ES31" s="37"/>
+      <c r="ET31" s="37"/>
+      <c r="EU31" s="37"/>
+      <c r="EV31" s="37"/>
+      <c r="EW31" s="37"/>
+      <c r="EX31" s="37"/>
+      <c r="EY31" s="37"/>
     </row>
     <row r="32" spans="1:240">
-      <c r="EM32" s="33" t="s">
+      <c r="EM32" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="EN32" s="33"/>
-      <c r="EO32" s="33"/>
-      <c r="EP32" s="33"/>
-      <c r="EQ32" s="33"/>
-      <c r="ER32" s="33"/>
-      <c r="ES32" s="33"/>
-      <c r="ET32" s="33"/>
-      <c r="EU32" s="33"/>
-      <c r="EV32" s="33"/>
-      <c r="EW32" s="33"/>
-      <c r="EX32" s="33"/>
-      <c r="EY32" s="33"/>
+      <c r="EN32" s="37"/>
+      <c r="EO32" s="37"/>
+      <c r="EP32" s="37"/>
+      <c r="EQ32" s="37"/>
+      <c r="ER32" s="37"/>
+      <c r="ES32" s="37"/>
+      <c r="ET32" s="37"/>
+      <c r="EU32" s="37"/>
+      <c r="EV32" s="37"/>
+      <c r="EW32" s="37"/>
+      <c r="EX32" s="37"/>
+      <c r="EY32" s="37"/>
     </row>
     <row r="33" spans="143:155">
-      <c r="EM33" s="33" t="s">
+      <c r="EM33" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="EN33" s="33"/>
-      <c r="EO33" s="33"/>
-      <c r="EP33" s="33"/>
-      <c r="EQ33" s="33"/>
-      <c r="ER33" s="33"/>
-      <c r="ES33" s="33"/>
-      <c r="ET33" s="33"/>
-      <c r="EU33" s="33"/>
-      <c r="EV33" s="33"/>
-      <c r="EW33" s="33"/>
-      <c r="EX33" s="33"/>
-      <c r="EY33" s="33"/>
+      <c r="EN33" s="37"/>
+      <c r="EO33" s="37"/>
+      <c r="EP33" s="37"/>
+      <c r="EQ33" s="37"/>
+      <c r="ER33" s="37"/>
+      <c r="ES33" s="37"/>
+      <c r="ET33" s="37"/>
+      <c r="EU33" s="37"/>
+      <c r="EV33" s="37"/>
+      <c r="EW33" s="37"/>
+      <c r="EX33" s="37"/>
+      <c r="EY33" s="37"/>
     </row>
     <row r="34" spans="143:155">
-      <c r="EM34" s="33" t="s">
+      <c r="EM34" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="EN34" s="33"/>
-      <c r="EO34" s="33"/>
-      <c r="EP34" s="33"/>
-      <c r="EQ34" s="33"/>
-      <c r="ER34" s="33"/>
-      <c r="ES34" s="33"/>
-      <c r="ET34" s="33"/>
-      <c r="EU34" s="33"/>
-      <c r="EV34" s="33"/>
-      <c r="EW34" s="33"/>
-      <c r="EX34" s="33"/>
-      <c r="EY34" s="33"/>
+      <c r="EN34" s="37"/>
+      <c r="EO34" s="37"/>
+      <c r="EP34" s="37"/>
+      <c r="EQ34" s="37"/>
+      <c r="ER34" s="37"/>
+      <c r="ES34" s="37"/>
+      <c r="ET34" s="37"/>
+      <c r="EU34" s="37"/>
+      <c r="EV34" s="37"/>
+      <c r="EW34" s="37"/>
+      <c r="EX34" s="37"/>
+      <c r="EY34" s="37"/>
     </row>
     <row r="35" spans="143:155">
-      <c r="EM35" s="33" t="s">
+      <c r="EM35" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="EN35" s="33"/>
-      <c r="EO35" s="33"/>
-      <c r="EP35" s="33"/>
-      <c r="EQ35" s="33"/>
-      <c r="ER35" s="33"/>
-      <c r="ES35" s="33"/>
-      <c r="ET35" s="33"/>
-      <c r="EU35" s="33"/>
-      <c r="EV35" s="33"/>
-      <c r="EW35" s="33"/>
-      <c r="EX35" s="33"/>
-      <c r="EY35" s="33"/>
+      <c r="EN35" s="37"/>
+      <c r="EO35" s="37"/>
+      <c r="EP35" s="37"/>
+      <c r="EQ35" s="37"/>
+      <c r="ER35" s="37"/>
+      <c r="ES35" s="37"/>
+      <c r="ET35" s="37"/>
+      <c r="EU35" s="37"/>
+      <c r="EV35" s="37"/>
+      <c r="EW35" s="37"/>
+      <c r="EX35" s="37"/>
+      <c r="EY35" s="37"/>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="S1:W1"/>
-    <mergeCell ref="X1:Z1"/>
-    <mergeCell ref="I2:N2"/>
-    <mergeCell ref="I1:N1"/>
-    <mergeCell ref="O1:Q1"/>
-    <mergeCell ref="O2:Q2"/>
-    <mergeCell ref="C4:AB4"/>
-    <mergeCell ref="AC4:BF4"/>
-    <mergeCell ref="BG4:CK4"/>
-    <mergeCell ref="CL4:DO4"/>
-    <mergeCell ref="DP4:ET4"/>
+    <mergeCell ref="EM31:EY31"/>
+    <mergeCell ref="EM32:EY32"/>
+    <mergeCell ref="EM33:EY33"/>
+    <mergeCell ref="EM34:EY34"/>
+    <mergeCell ref="EM35:EY35"/>
+    <mergeCell ref="EM30:EY30"/>
+    <mergeCell ref="EM19:EY19"/>
+    <mergeCell ref="EM20:EY20"/>
+    <mergeCell ref="EM21:EY21"/>
+    <mergeCell ref="EM22:EY22"/>
+    <mergeCell ref="EM23:EY23"/>
+    <mergeCell ref="EM24:EY24"/>
+    <mergeCell ref="EM25:EY25"/>
+    <mergeCell ref="EM26:EY26"/>
+    <mergeCell ref="EM27:EY27"/>
+    <mergeCell ref="EM28:EY28"/>
+    <mergeCell ref="EM29:EY29"/>
     <mergeCell ref="EM18:EY18"/>
     <mergeCell ref="FZ4:HA4"/>
     <mergeCell ref="HB4:IF4"/>
@@ -4374,23 +4443,17 @@
     <mergeCell ref="EM15:EY15"/>
     <mergeCell ref="EM16:EY16"/>
     <mergeCell ref="EM17:EY17"/>
-    <mergeCell ref="EM30:EY30"/>
-    <mergeCell ref="EM19:EY19"/>
-    <mergeCell ref="EM20:EY20"/>
-    <mergeCell ref="EM21:EY21"/>
-    <mergeCell ref="EM22:EY22"/>
-    <mergeCell ref="EM23:EY23"/>
-    <mergeCell ref="EM24:EY24"/>
-    <mergeCell ref="EM25:EY25"/>
-    <mergeCell ref="EM26:EY26"/>
-    <mergeCell ref="EM27:EY27"/>
-    <mergeCell ref="EM28:EY28"/>
-    <mergeCell ref="EM29:EY29"/>
-    <mergeCell ref="EM31:EY31"/>
-    <mergeCell ref="EM32:EY32"/>
-    <mergeCell ref="EM33:EY33"/>
-    <mergeCell ref="EM34:EY34"/>
-    <mergeCell ref="EM35:EY35"/>
+    <mergeCell ref="C4:AB4"/>
+    <mergeCell ref="AC4:BF4"/>
+    <mergeCell ref="BG4:CK4"/>
+    <mergeCell ref="CL4:DO4"/>
+    <mergeCell ref="DP4:ET4"/>
+    <mergeCell ref="S1:W1"/>
+    <mergeCell ref="X1:Z1"/>
+    <mergeCell ref="I2:N2"/>
+    <mergeCell ref="I1:N1"/>
+    <mergeCell ref="O1:Q1"/>
+    <mergeCell ref="O2:Q2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>